<commit_message>
Add properly linked list structure
</commit_message>
<xml_diff>
--- a/circ_link_list/diagram_of_cllist.xlsx
+++ b/circ_link_list/diagram_of_cllist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gytis\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gytis\Desktop\code\rv32i-course\circ_link_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{119ECDB3-16A9-474C-BFF0-86570EE3861C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D18B47-D572-4ACF-98C8-765A2CAC778C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F55825A-3D38-4A5F-A1A2-11A4DF357CE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="10">
   <si>
     <t>node1</t>
   </si>
@@ -72,17 +72,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,21 +96,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9"/>
+      <color rgb="FFFFFF00"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -125,16 +136,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,222 +542,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37B8C87-3914-4560-AFC9-537E10217A58}">
-  <dimension ref="E6:I25"/>
+  <dimension ref="A6:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H6" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="G6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="7" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="G7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="G8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="L8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="V8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="2" t="s">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="V10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y10" s="1"/>
     </row>
-    <row r="12" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="2" t="s">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="W11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X11" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" s="1" t="s">
+      <c r="Y11" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>